<commit_message>
Commit 5 : amelioration import transactions
</commit_message>
<xml_diff>
--- a/achat_ETF_et_fonds_actions_commodities.xlsx
+++ b/achat_ETF_et_fonds_actions_commodities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seble\Code\env\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2A0656-7883-4E76-8E06-AB6985E9BC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03954A30-7F7B-4A3A-8B1A-12CFBE73FD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4370" yWindow="7830" windowWidth="24710" windowHeight="8440" xr2:uid="{AD1E8AB5-6CC3-47BD-96C0-94E38042B0ED}"/>
+    <workbookView xWindow="2150" yWindow="8240" windowWidth="24710" windowHeight="8440" xr2:uid="{AD1E8AB5-6CC3-47BD-96C0-94E38042B0ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
   <si>
     <t>Isin</t>
   </si>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0EA90D-9F81-42CE-8D17-9B6578B34CEC}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="49.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>46063</v>
+        <v>46070</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>46066</v>
+        <v>46063</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -548,10 +548,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -562,24 +562,162 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
+        <v>46066</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>46068</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>46073</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>40</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>46069</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
         <v>40</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E7" s="2">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>50</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>46075</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>50</v>
+      </c>
+      <c r="E9" s="2">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>46079</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>